<commit_message>
Updated Backlog.xlsx and added Player Buttons in activity_overview.xml
</commit_message>
<xml_diff>
--- a/Documentation/Backlog.xlsx
+++ b/Documentation/Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
   <si>
     <t>Task</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>Architecture Slide</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -517,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +536,7 @@
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -543,8 +549,11 @@
       <c r="D1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -552,7 +561,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -563,7 +572,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -574,7 +583,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -585,7 +594,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -596,7 +605,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -607,7 +616,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -618,7 +627,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -629,7 +638,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -640,7 +649,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -651,7 +660,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -662,7 +671,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -673,7 +682,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -684,7 +693,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -694,11 +703,11 @@
       <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -706,7 +715,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -714,7 +723,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -722,7 +731,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -730,7 +739,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -741,7 +750,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -752,7 +761,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -763,15 +772,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -779,7 +791,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -787,15 +799,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
       <c r="C26" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -803,7 +818,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -811,7 +826,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -819,18 +834,18 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
       <c r="C30" t="s">
         <v>53</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -838,14 +853,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
       <c r="C32" t="s">
         <v>53</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Backlog and Images Excel. Added 10 paintings in firebase
</commit_message>
<xml_diff>
--- a/Documentation/Backlog.xlsx
+++ b/Documentation/Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Dropbox\000_KTH\10_Courses\P3\DH2642_Programming\Project\DH2642\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\GitHub\DH2642\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
   <si>
     <t>Task</t>
   </si>
@@ -198,13 +198,22 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Add Image Reference</t>
+  </si>
+  <si>
+    <t>Images and Descriptions from National Gallery of Art http://www.nga.gov/</t>
+  </si>
+  <si>
+    <t>Add Images in Firebase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,13 +228,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -240,9 +263,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,19 +562,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>56</v>
       </c>
     </row>
@@ -864,7 +889,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -872,7 +897,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -880,7 +905,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -888,7 +913,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -896,7 +921,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -904,7 +929,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -912,32 +937,57 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>

</xml_diff>